<commit_message>
Commit9.0.184- finalização candidatos- 14
</commit_message>
<xml_diff>
--- a/documentos/Algoritmos/Algoritmos2.xlsx
+++ b/documentos/Algoritmos/Algoritmos2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Manutenção" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>iViewSudokuBoard</t>
   </si>
@@ -81,13 +81,40 @@
     <t>M25</t>
   </si>
   <si>
-    <t>1- "Volta Jogo"</t>
-  </si>
-  <si>
     <t>4- "Volta Jogo": NÃO OK!</t>
   </si>
   <si>
-    <t>#406 breakpoint</t>
+    <t>Classe JogarActivity</t>
+  </si>
+  <si>
+    <t>#276 analisaCandidatos</t>
+  </si>
+  <si>
+    <t>#526 analisaCandidatos</t>
+  </si>
+  <si>
+    <t>M20</t>
+  </si>
+  <si>
+    <t>1- "iViewSudokuBoard" toque</t>
+  </si>
+  <si>
+    <t>2- "iViewNumsDisps" toque</t>
+  </si>
+  <si>
+    <t>2.1- "Volta Jogo"</t>
+  </si>
+  <si>
+    <t>2.2- #298    iViewNumsDisps!!.setOnTouchListener</t>
+  </si>
+  <si>
+    <t>2.3- #1955 analisaCandidatos</t>
+  </si>
+  <si>
+    <t>#216</t>
+  </si>
+  <si>
+    <t>#404</t>
   </si>
 </sst>
 </file>
@@ -299,26 +326,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -331,21 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -356,6 +350,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,91 +693,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:12">
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="C5" s="11"/>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="1" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="13"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="13"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C7" s="11"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="13"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="17"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="11" spans="2:12">
       <c r="C11" t="s">
@@ -755,241 +785,241 @@
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C14" s="11"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="C15" s="11"/>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="1" t="s">
+      <c r="E15" s="20"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="13"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="12"/>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12" t="s">
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="13"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" thickBot="1">
-      <c r="C17" s="11"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="13"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12" t="s">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12" t="s">
+      <c r="J20" s="6"/>
+      <c r="K20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="13"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="7"/>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="25" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12" t="s">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12" t="s">
+      <c r="J21" s="6"/>
+      <c r="K21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="13"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="13"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="13"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="26" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="13"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="26" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="13"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="26" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="13"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="7"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="C27" s="11"/>
-      <c r="D27" s="28" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="13"/>
+      <c r="E27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="I29" s="29"/>
+      <c r="I29" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1005,34 +1035,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:B7"/>
+  <dimension ref="C2:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:2">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
+    <row r="2" spans="3:3">
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3">
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3">
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="3:3">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" s="30" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
+      <c r="C16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Commit9.0.185- finalização candidatos- 15
- final da implementação dos Candidatos
- início de tentativa de ter solução UNIQUE
</commit_message>
<xml_diff>
--- a/documentos/Algoritmos/Algoritmos2.xlsx
+++ b/documentos/Algoritmos/Algoritmos2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Manutenção" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>iViewSudokuBoard</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Classe JogarActivity</t>
   </si>
   <si>
-    <t>#276 analisaCandidatos</t>
-  </si>
-  <si>
-    <t>#526 analisaCandidatos</t>
-  </si>
-  <si>
     <t>M20</t>
   </si>
   <si>
@@ -108,13 +102,34 @@
     <t>2.2- #298    iViewNumsDisps!!.setOnTouchListener</t>
   </si>
   <si>
-    <t>2.3- #1955 analisaCandidatos</t>
-  </si>
-  <si>
     <t>#216</t>
   </si>
   <si>
     <t>#404</t>
+  </si>
+  <si>
+    <t>#280 analisaCandidatos</t>
+  </si>
+  <si>
+    <t>#530 analisaCandidatos</t>
+  </si>
+  <si>
+    <t>#530 - iViewNumsDisps!!.setOnTouchListener</t>
+  </si>
+  <si>
+    <t>#580 - btnCand.setOnClickListener</t>
+  </si>
+  <si>
+    <t>#968 - mostraNumsIguais</t>
+  </si>
+  <si>
+    <t>2.3- #1963 analisaCandidatos</t>
+  </si>
+  <si>
+    <t>#270 - mostraCelAJogar</t>
+  </si>
+  <si>
+    <t>#217 - iViewSudokuBoard!!.setOnTouchListener</t>
   </si>
 </sst>
 </file>
@@ -350,6 +365,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,9 +400,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,44 +742,44 @@
     </row>
     <row r="5" spans="2:12">
       <c r="C5" s="5"/>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="20"/>
+      <c r="K5" s="21"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="2:12">
       <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1">
       <c r="C7" s="5"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="2:12">
@@ -826,18 +841,18 @@
     </row>
     <row r="15" spans="2:12">
       <c r="C15" s="5"/>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="25"/>
+      <c r="K15" s="26"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="2:12">
@@ -845,28 +860,28 @@
       <c r="C16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" thickBot="1">
       <c r="C17" s="5"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12">
@@ -1035,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:C16"/>
+  <dimension ref="C2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,7 +1064,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="3:3">
@@ -1059,22 +1074,22 @@
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="3:3">
@@ -1082,27 +1097,52 @@
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="30" t="s">
-        <v>23</v>
+      <c r="C13" s="19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="3:3">
-      <c r="C14" s="30" t="s">
-        <v>24</v>
+      <c r="C14" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>